<commit_message>
Updated router import xlsx
</commit_message>
<xml_diff>
--- a/bothub/common/static/bothub/exporter/example.xlsx
+++ b/bothub/common/static/bothub/exporter/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Entities</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Translate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translation Error</t>
   </si>
 </sst>
 </file>
@@ -306,13 +309,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.32"/>
@@ -320,6 +323,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="49.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -395,6 +399,9 @@
       </c>
       <c r="F13" s="11" t="s">
         <v>9</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>